<commit_message>
updated excel file and rdata to get rid of duplicate ATBC.
</commit_message>
<xml_diff>
--- a/inst/extdata/cohorts.xlsx
+++ b/inst/extdata/cohorts.xlsx
@@ -1,22 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayca\OneDrive\Documents\Ella\COMETSAnalytics\inst\extdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="48" windowWidth="20112" windowHeight="7992"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$34</definedName>
+  </definedNames>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Cohort</t>
   </si>
@@ -126,8 +134,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,6 +173,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -211,7 +227,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -243,9 +259,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -277,6 +311,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -452,20 +504,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -473,302 +525,299 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1">
+        <v>42620</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1">
-        <v>42620</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="B3" s="1">
+        <v>42620</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1">
+        <v>42620</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="1">
+        <v>42620</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1">
+        <v>42620</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1">
+        <v>42620</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="1">
+        <v>42620</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="1">
+        <v>42620</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1">
+        <v>42620</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="1">
+        <v>42620</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="1">
+        <v>42620</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="1">
+        <v>42620</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="1">
+        <v>42620</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1">
+        <v>42620</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="1">
+        <v>42620</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="1">
+        <v>42620</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1">
-        <v>42620</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
-        <v>42620</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+      <c r="B18" s="1">
+        <v>42620</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="1">
+        <v>42620</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="1">
+        <v>42620</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="1">
+        <v>42620</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="1">
+        <v>42620</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="1">
+        <v>42620</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="1">
+        <v>42620</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1">
+        <v>42620</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1">
+        <v>42620</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="1">
+        <v>42620</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="1">
+        <v>42620</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="1">
+        <v>42620</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1">
+        <v>42620</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="1">
+        <v>42620</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1">
-        <v>42620</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1">
-        <v>42620</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1">
-        <v>42620</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1">
-        <v>42620</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="1">
-        <v>42620</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="1">
-        <v>42620</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="1">
-        <v>42620</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="1">
-        <v>42620</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="1">
-        <v>42620</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="1">
-        <v>42620</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
+      <c r="B32" s="1">
+        <v>42620</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="1">
-        <v>42620</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="1">
-        <v>42620</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="1">
-        <v>42620</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="1">
-        <v>42620</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="1">
-        <v>42620</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="1">
-        <v>42620</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="1">
-        <v>42620</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="1">
-        <v>42620</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="1">
-        <v>42620</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="1">
-        <v>42620</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" s="1">
-        <v>42620</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
+      <c r="B33" s="1">
+        <v>42620</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="1">
-        <v>42620</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" s="1">
-        <v>42620</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" s="1">
-        <v>42620</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" s="1">
-        <v>42620</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="1">
-        <v>42620</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" s="1">
-        <v>42620</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" t="s">
-        <v>2</v>
-      </c>
-      <c r="B32" s="1">
-        <v>42620</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33" s="1">
-        <v>42620</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" t="s">
-        <v>33</v>
-      </c>
       <c r="B34" s="1">
         <v>42620</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
-      <c r="A35" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" s="1">
-        <v>42620</v>
-      </c>
-    </row>
   </sheetData>
+  <autoFilter ref="A1:B34">
+    <sortState ref="A2:B35">
+      <sortCondition ref="A2:A35"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>